<commit_message>
sensei ni kiita ato
</commit_message>
<xml_diff>
--- a/documents/内部設計/061625_03_ファイル構成一覧表_A5.xlsx
+++ b/documents/内部設計/061625_03_ファイル構成一覧表_A5.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\plusdojo2025\A5\documents\内部設計\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89B0A748-928C-4A25-9CE3-EFB0D0D727FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D95064AE-5B43-4ED0-ADA0-A1165BE7FFBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11640" yWindow="7200" windowWidth="36900" windowHeight="23445" xr2:uid="{8AE99860-7ADF-4316-9590-B2AD2D1E8F62}"/>
+    <workbookView xWindow="20100" yWindow="8040" windowWidth="36900" windowHeight="23445" xr2:uid="{8AE99860-7ADF-4316-9590-B2AD2D1E8F62}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$C$2:$N$60</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -2780,6 +2781,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="ドキュメント" ma:contentTypeID="0x010100157231BE4AEE574CA53F7F6406B00885" ma:contentTypeVersion="5" ma:contentTypeDescription="新しいドキュメントを作成します。" ma:contentTypeScope="" ma:versionID="dc5b9a23ce3d52c4956bed0e463d1dda">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="f11e5c67-cf10-45fe-9586-3550a4dd026c" xmlns:ns4="01c64581-d9a7-4bf3-8493-a30fa4f21230" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7c0a2f94ac7d166380f87837b42de16b" ns3:_="" ns4:_="">
     <xsd:import namespace="f11e5c67-cf10-45fe-9586-3550a4dd026c"/>
@@ -2950,12 +2957,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -2966,6 +2967,23 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2CD51129-CE6F-45E1-BB00-4EFAA7AA477C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="01c64581-d9a7-4bf3-8493-a30fa4f21230"/>
+    <ds:schemaRef ds:uri="f11e5c67-cf10-45fe-9586-3550a4dd026c"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A480FB52-0471-4E93-ADEA-9D5C32C7BB5B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2984,23 +3002,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2CD51129-CE6F-45E1-BB00-4EFAA7AA477C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="01c64581-d9a7-4bf3-8493-a30fa4f21230"/>
-    <ds:schemaRef ds:uri="f11e5c67-cf10-45fe-9586-3550a4dd026c"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39FADF03-5109-4CCE-A5D7-74DA56792023}">
   <ds:schemaRefs>

</xml_diff>